<commit_message>
fix error in order form
</commit_message>
<xml_diff>
--- a/public/files/aaup/AAUP_Data_15-16_Order_Form.xlsx
+++ b/public/files/aaup/AAUP_Data_15-16_Order_Form.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8265" windowHeight="4650"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="6" r:id="rId1"/>
@@ -9537,9 +9537,6 @@
   </si>
   <si>
     <t>There are eight different report formats available. Each report compares a basis institution to a set of peer institutions you will choose. Please see the PCR Instructions tab for complete ordering information.  All of these data are available via the Results Portal.</t>
-  </si>
-  <si>
-    <t>The Results Portal you acess to our online results portal which allows you to create and save your own peer lists and create fully customizable on specific variables not included in peer compensation reports.</t>
   </si>
   <si>
     <t xml:space="preserve">This includes many options for custom data vizualization of bar charts, scatterplots, and multiple options for exporting data. </t>
@@ -9843,6 +9840,9 @@
   </si>
   <si>
     <t>Requested By:</t>
+  </si>
+  <si>
+    <t>The Results Portal provides allows you to create and save your own peer lists and create fully customizable analyses on specific variables not included in peer compensation reports.</t>
   </si>
 </sst>
 </file>
@@ -10505,6 +10505,9 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -10525,9 +10528,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -11038,12 +11038,12 @@
     <row r="8" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="9" spans="1:15" s="14" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>3164</v>
+        <v>3163</v>
       </c>
     </row>
     <row r="10" spans="1:15" s="79" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>3178</v>
+        <v>3177</v>
       </c>
       <c r="B10" s="15"/>
       <c r="C10" s="16"/>
@@ -11059,7 +11059,7 @@
     <row r="11" spans="1:15" s="79" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="17"/>
       <c r="B11" s="82" t="s">
-        <v>3161</v>
+        <v>3187</v>
       </c>
       <c r="C11" s="82"/>
       <c r="D11" s="82"/>
@@ -11073,12 +11073,12 @@
     </row>
     <row r="12" spans="1:15" s="79" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="79" t="s">
-        <v>3162</v>
+        <v>3161</v>
       </c>
     </row>
     <row r="13" spans="1:15" s="79" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="79" t="s">
-        <v>3163</v>
+        <v>3162</v>
       </c>
     </row>
     <row r="14" spans="1:15" s="14" customFormat="1" ht="14.25" x14ac:dyDescent="0.2"/>
@@ -11090,7 +11090,7 @@
     </row>
     <row r="16" spans="1:15" s="14" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="82" t="s">
-        <v>3186</v>
+        <v>3185</v>
       </c>
       <c r="C16" s="82"/>
       <c r="D16" s="82"/>
@@ -11105,13 +11105,13 @@
     <row r="17" spans="1:11" s="14" customFormat="1" ht="14.25" x14ac:dyDescent="0.2"/>
     <row r="18" spans="1:11" s="16" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
-        <v>3179</v>
+        <v>3178</v>
       </c>
       <c r="B18" s="15"/>
     </row>
     <row r="19" spans="1:11" s="14" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B19" s="83" t="s">
-        <v>3176</v>
+        <v>3175</v>
       </c>
       <c r="C19" s="83"/>
       <c r="D19" s="83"/>
@@ -11125,7 +11125,7 @@
     </row>
     <row r="21" spans="1:11" s="15" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
-        <v>3180</v>
+        <v>3179</v>
       </c>
     </row>
     <row r="22" spans="1:11" s="14" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -11204,7 +11204,7 @@
     </row>
     <row r="10" spans="1:2" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
-        <v>3187</v>
+        <v>3186</v>
       </c>
       <c r="B10" s="80"/>
     </row>
@@ -11344,7 +11344,7 @@
     </row>
     <row r="6" spans="1:6" s="10" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
-        <v>3184</v>
+        <v>3183</v>
       </c>
       <c r="B6" s="18"/>
       <c r="C6" s="18"/>
@@ -11376,7 +11376,7 @@
         <v>1000</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>3185</v>
+        <v>3184</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -11581,7 +11581,7 @@
     <row r="8" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="29"/>
       <c r="B8" s="52" t="s">
-        <v>3167</v>
+        <v>3166</v>
       </c>
       <c r="C8" s="53"/>
       <c r="E8" s="53"/>
@@ -11590,25 +11590,25 @@
     </row>
     <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="53"/>
-      <c r="B9" s="88" t="s">
+      <c r="B9" s="89" t="s">
         <v>2951</v>
       </c>
-      <c r="C9" s="88"/>
+      <c r="C9" s="89"/>
       <c r="D9" s="54"/>
-      <c r="E9" s="92"/>
-      <c r="F9" s="92"/>
+      <c r="E9" s="93"/>
+      <c r="F9" s="93"/>
     </row>
     <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="89" t="s">
+      <c r="A10" s="90" t="s">
         <v>2959</v>
       </c>
-      <c r="B10" s="93" t="s">
+      <c r="B10" s="94" t="s">
         <v>3154</v>
       </c>
-      <c r="C10" s="94"/>
+      <c r="C10" s="95"/>
     </row>
     <row r="11" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="89"/>
+      <c r="A11" s="90"/>
       <c r="B11" s="55"/>
       <c r="C11" s="56"/>
       <c r="D11" s="57"/>
@@ -11617,16 +11617,16 @@
       <c r="A12" s="58" t="s">
         <v>3155</v>
       </c>
-      <c r="B12" s="90">
+      <c r="B12" s="91">
         <v>450</v>
       </c>
-      <c r="C12" s="90"/>
+      <c r="C12" s="91"/>
       <c r="D12" s="59"/>
     </row>
     <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="60"/>
-      <c r="B13" s="91"/>
-      <c r="C13" s="91"/>
+      <c r="B13" s="92"/>
+      <c r="C13" s="92"/>
       <c r="D13" s="59"/>
     </row>
     <row r="14" spans="1:7" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -11654,95 +11654,101 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="95" t="s">
+      <c r="A20" s="88" t="s">
+        <v>3167</v>
+      </c>
+      <c r="B20" s="88"/>
+      <c r="C20" s="88"/>
+      <c r="D20" s="88"/>
+      <c r="E20" s="88"/>
+      <c r="F20" s="88"/>
+      <c r="G20" s="88"/>
+    </row>
+    <row r="21" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="88" t="s">
         <v>3168</v>
       </c>
-      <c r="B20" s="95"/>
-      <c r="C20" s="95"/>
-      <c r="D20" s="95"/>
-      <c r="E20" s="95"/>
-      <c r="F20" s="95"/>
-      <c r="G20" s="95"/>
-    </row>
-    <row r="21" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="95" t="s">
+      <c r="B21" s="88"/>
+      <c r="C21" s="88"/>
+      <c r="D21" s="88"/>
+      <c r="E21" s="88"/>
+      <c r="F21" s="88"/>
+      <c r="G21" s="88"/>
+    </row>
+    <row r="22" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="88" t="s">
         <v>3169</v>
       </c>
-      <c r="B21" s="95"/>
-      <c r="C21" s="95"/>
-      <c r="D21" s="95"/>
-      <c r="E21" s="95"/>
-      <c r="F21" s="95"/>
-      <c r="G21" s="95"/>
-    </row>
-    <row r="22" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="95" t="s">
-        <v>3170</v>
-      </c>
-      <c r="B22" s="95"/>
-      <c r="C22" s="95"/>
-      <c r="D22" s="95"/>
-      <c r="E22" s="95"/>
-      <c r="F22" s="95"/>
-      <c r="G22" s="95"/>
+      <c r="B22" s="88"/>
+      <c r="C22" s="88"/>
+      <c r="D22" s="88"/>
+      <c r="E22" s="88"/>
+      <c r="F22" s="88"/>
+      <c r="G22" s="88"/>
     </row>
     <row r="23" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="95" t="s">
-        <v>3177</v>
-      </c>
-      <c r="B23" s="95"/>
-      <c r="C23" s="95"/>
-      <c r="D23" s="95"/>
-      <c r="E23" s="95"/>
-      <c r="F23" s="95"/>
-      <c r="G23" s="95"/>
+      <c r="A23" s="88" t="s">
+        <v>3176</v>
+      </c>
+      <c r="B23" s="88"/>
+      <c r="C23" s="88"/>
+      <c r="D23" s="88"/>
+      <c r="E23" s="88"/>
+      <c r="F23" s="88"/>
+      <c r="G23" s="88"/>
     </row>
     <row r="24" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="95" t="s">
+      <c r="A24" s="88" t="s">
+        <v>3171</v>
+      </c>
+      <c r="B24" s="88"/>
+      <c r="C24" s="88"/>
+      <c r="D24" s="88"/>
+      <c r="E24" s="88"/>
+      <c r="F24" s="88"/>
+      <c r="G24" s="88"/>
+    </row>
+    <row r="25" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="88" t="s">
         <v>3172</v>
       </c>
-      <c r="B24" s="95"/>
-      <c r="C24" s="95"/>
-      <c r="D24" s="95"/>
-      <c r="E24" s="95"/>
-      <c r="F24" s="95"/>
-      <c r="G24" s="95"/>
-    </row>
-    <row r="25" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="95" t="s">
+      <c r="B25" s="88"/>
+      <c r="C25" s="88"/>
+      <c r="D25" s="88"/>
+      <c r="E25" s="88"/>
+      <c r="F25" s="88"/>
+      <c r="G25" s="88"/>
+    </row>
+    <row r="26" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="88" t="s">
         <v>3173</v>
       </c>
-      <c r="B25" s="95"/>
-      <c r="C25" s="95"/>
-      <c r="D25" s="95"/>
-      <c r="E25" s="95"/>
-      <c r="F25" s="95"/>
-      <c r="G25" s="95"/>
-    </row>
-    <row r="26" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="95" t="s">
+      <c r="B26" s="88"/>
+      <c r="C26" s="88"/>
+      <c r="D26" s="88"/>
+      <c r="E26" s="88"/>
+      <c r="F26" s="88"/>
+      <c r="G26" s="88"/>
+    </row>
+    <row r="27" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="88" t="s">
         <v>3174</v>
       </c>
-      <c r="B26" s="95"/>
-      <c r="C26" s="95"/>
-      <c r="D26" s="95"/>
-      <c r="E26" s="95"/>
-      <c r="F26" s="95"/>
-      <c r="G26" s="95"/>
-    </row>
-    <row r="27" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="95" t="s">
-        <v>3175</v>
-      </c>
-      <c r="B27" s="95"/>
-      <c r="C27" s="95"/>
-      <c r="D27" s="95"/>
-      <c r="E27" s="95"/>
-      <c r="F27" s="95"/>
-      <c r="G27" s="95"/>
+      <c r="B27" s="88"/>
+      <c r="C27" s="88"/>
+      <c r="D27" s="88"/>
+      <c r="E27" s="88"/>
+      <c r="F27" s="88"/>
+      <c r="G27" s="88"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="B10:C10"/>
     <mergeCell ref="A24:G24"/>
     <mergeCell ref="A25:G25"/>
     <mergeCell ref="A26:G26"/>
@@ -11751,12 +11757,6 @@
     <mergeCell ref="A21:G21"/>
     <mergeCell ref="A22:G22"/>
     <mergeCell ref="A23:G23"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="B10:C10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup scale="92" orientation="landscape" r:id="rId1"/>
@@ -11802,7 +11802,7 @@
     </row>
     <row r="6" spans="1:1" s="14" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>3166</v>
+        <v>3165</v>
       </c>
     </row>
     <row r="7" spans="1:1" s="14" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -11847,7 +11847,7 @@
     </row>
     <row r="17" spans="1:4" s="16" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
-        <v>3182</v>
+        <v>3181</v>
       </c>
     </row>
     <row r="18" spans="1:4" s="14" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
@@ -11857,14 +11857,14 @@
     </row>
     <row r="19" spans="1:4" s="14" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A19" s="14" t="s">
-        <v>3183</v>
+        <v>3182</v>
       </c>
     </row>
     <row r="20" spans="1:4" s="14" customFormat="1" ht="14.25" x14ac:dyDescent="0.2"/>
     <row r="21" spans="1:4" s="14" customFormat="1" ht="14.25" x14ac:dyDescent="0.2"/>
     <row r="22" spans="1:4" s="16" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
-        <v>3165</v>
+        <v>3164</v>
       </c>
     </row>
     <row r="23" spans="1:4" s="14" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
@@ -11915,7 +11915,7 @@
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A46" sqref="A46"/>
-      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -11971,7 +11971,7 @@
       <c r="C5" s="6"/>
       <c r="D5" s="43"/>
       <c r="F5" s="34" t="s">
-        <v>3181</v>
+        <v>3180</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -13173,7 +13173,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="45" t="s">
-        <v>3171</v>
+        <v>3170</v>
       </c>
       <c r="B3" s="47"/>
       <c r="C3" s="47"/>

</xml_diff>